<commit_message>
Updated code with invalid login and workday downtime handling
</commit_message>
<xml_diff>
--- a/Input/UserDetails.xlsx
+++ b/Input/UserDetails.xlsx
@@ -1,142 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibmadmin\PycharmProjects\Workday\Input\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCE19FC-5803-476C-9E35-5D61C3062447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="shiftDetails" sheetId="2" r:id="rId2"/>
-    <sheet name="vacation" sheetId="3" r:id="rId3"/>
+    <sheet name="loginDetails" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="shiftDetails" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="vacation" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Avik Datta</t>
-  </si>
-  <si>
-    <t>avdatta2@in.ibm.com</t>
-  </si>
-  <si>
-    <t>./Input/secret.txt</t>
-  </si>
-  <si>
-    <t>Shift</t>
-  </si>
-  <si>
-    <t>Sat</t>
-  </si>
-  <si>
-    <t>Sun</t>
-  </si>
-  <si>
-    <t>Mon</t>
-  </si>
-  <si>
-    <t>Tue</t>
-  </si>
-  <si>
-    <t>Wed</t>
-  </si>
-  <si>
-    <t>Thu</t>
-  </si>
-  <si>
-    <t>Fri</t>
-  </si>
-  <si>
-    <t>Shift 2</t>
-  </si>
-  <si>
-    <t>Beginning Year Balance</t>
-  </si>
-  <si>
-    <t>Carryover Balance</t>
-  </si>
-  <si>
-    <t>Accrued Year To Date</t>
-  </si>
-  <si>
-    <t>Absence Paid Year To Date</t>
-  </si>
-  <si>
-    <t>Beginning Period Balance</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Inherit"/>
+      <b val="1"/>
+      <color rgb="FF333333"/>
       <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -149,12 +64,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.1499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -172,6 +93,86 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -182,35 +183,131 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="24">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -510,111 +607,174 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col width="14.453125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="19.453125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="15.26953125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Avik Datta</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>avdatta2@in.ibm.com</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>./Input/secret.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="E4" s="16" t="inlineStr">
+        <is>
+          <t>Create a secret.txt file inside Input folder and keep your password there. Please ensure secret.txt is added to gitignore file to avoid upload</t>
+        </is>
+      </c>
+      <c r="F4" s="17" t="n"/>
+      <c r="G4" s="17" t="n"/>
+      <c r="H4" s="17" t="n"/>
+      <c r="I4" s="18" t="n"/>
+    </row>
+    <row r="5">
+      <c r="E5" s="19" t="n"/>
+      <c r="I5" s="20" t="n"/>
+    </row>
+    <row r="6">
+      <c r="E6" s="21" t="n"/>
+      <c r="F6" s="22" t="n"/>
+      <c r="G6" s="22" t="n"/>
+      <c r="H6" s="22" t="n"/>
+      <c r="I6" s="23" t="n"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E4:I6"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" paperSize="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="A1" sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>13</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Shift</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Mon</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3">
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>Shift 2</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -624,58 +784,82 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="A2:E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col width="11.36328125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="8.81640625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="11.1796875" customWidth="1" min="3" max="3"/>
+    <col width="12.36328125" customWidth="1" min="4" max="4"/>
+    <col width="13.81640625" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34.5" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>19</v>
+    <row r="1" ht="34.5" customHeight="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Beginning Year Balance</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Carryover Balance</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Accrued Year To Date</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Absence Paid Year To Date</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>Beginning Period Balance</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>24</v>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D2" s="6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" paperSize="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding script for recording absence.
</commit_message>
<xml_diff>
--- a/Input/UserDetails.xlsx
+++ b/Input/UserDetails.xlsx
@@ -1,57 +1,164 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibmadmin\PycharmProjects\Workday\Input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5F9F14-D533-4C61-9172-9B8688D05CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="loginDetails" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="shiftDetails" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="vacation" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="shiftDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="vacation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Avik Datta</t>
+  </si>
+  <si>
+    <t>avdatta2@in.ibm.com</t>
+  </si>
+  <si>
+    <t>./Input/secret.txt</t>
+  </si>
+  <si>
+    <t>Create a secret.txt file inside Input folder and keep your password there. Please ensure secret.txt is added to gitignore file to avoid upload</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>Sat</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Shift 2</t>
+  </si>
+  <si>
+    <t>Beginning Year Balance</t>
+  </si>
+  <si>
+    <t>Carryover Balance</t>
+  </si>
+  <si>
+    <t>Accrued Year To Date</t>
+  </si>
+  <si>
+    <t>Absence Paid Year To Date</t>
+  </si>
+  <si>
+    <t>Beginning Period Balance</t>
+  </si>
+  <si>
+    <t>Request Vacation Days</t>
+  </si>
+  <si>
+    <t>Vacation Start</t>
+  </si>
+  <si>
+    <t>Vacation End</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>June 22, 2022</t>
+  </si>
+  <si>
+    <t>June 23, 2022</t>
+  </si>
+  <si>
+    <t>Sample Date
+August 23, 2022</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
       <name val="Inherit"/>
-      <b val="1"/>
-      <color rgb="FF333333"/>
-      <sz val="9"/>
     </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -64,7 +171,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.1499984740745262"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -99,17 +206,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -176,6 +272,17 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -183,131 +290,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -607,174 +644,137 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col width="14.453125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="19.453125" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="15.26953125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col min="1" max="1" width="14.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Password</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>Avik Datta</t>
-        </is>
-      </c>
-      <c r="B2" s="4" t="inlineStr">
-        <is>
-          <t>avdatta2@in.ibm.com</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>./Input/secret.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="E4" s="16" t="inlineStr">
-        <is>
-          <t>Create a secret.txt file inside Input folder and keep your password there. Please ensure secret.txt is added to gitignore file to avoid upload</t>
-        </is>
-      </c>
-      <c r="F4" s="17" t="n"/>
-      <c r="G4" s="17" t="n"/>
-      <c r="H4" s="17" t="n"/>
-      <c r="I4" s="18" t="n"/>
-    </row>
-    <row r="5">
-      <c r="E5" s="19" t="n"/>
-      <c r="I5" s="20" t="n"/>
-    </row>
-    <row r="6">
-      <c r="E6" s="21" t="n"/>
-      <c r="F6" s="22" t="n"/>
-      <c r="G6" s="22" t="n"/>
-      <c r="H6" s="22" t="n"/>
-      <c r="I6" s="23" t="n"/>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="E4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E4:I6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:H2"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Shift</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Sat</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Sun</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Mon</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Tue</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Wed</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>Thu</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Fri</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>Shift 2</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="n">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="3">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" s="3">
         <v>1</v>
       </c>
     </row>
@@ -784,82 +784,91 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col width="11.36328125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="8.81640625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="11.1796875" customWidth="1" min="3" max="3"/>
-    <col width="12.36328125" customWidth="1" min="4" max="4"/>
-    <col width="13.81640625" customWidth="1" min="5" max="5"/>
+    <col min="1" max="1" width="11.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" style="7" customWidth="1"/>
+    <col min="7" max="8" width="12" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="34.5" customHeight="1">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>Beginning Year Balance</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>Carryover Balance</t>
-        </is>
-      </c>
-      <c r="C1" s="5" t="inlineStr">
-        <is>
-          <t>Accrued Year To Date</t>
-        </is>
-      </c>
-      <c r="D1" s="5" t="inlineStr">
-        <is>
-          <t>Absence Paid Year To Date</t>
-        </is>
-      </c>
-      <c r="E1" s="5" t="inlineStr">
-        <is>
-          <t>Beginning Period Balance</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="C2" s="6" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E2" s="6" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
+    <row r="1" spans="1:12" ht="34.5" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="J4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="J5" s="21"/>
+      <c r="K5" s="22"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J4:K5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Further updates to the script for recording absence.
</commit_message>
<xml_diff>
--- a/Input/UserDetails.xlsx
+++ b/Input/UserDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibmadmin\PycharmProjects\Workday\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54996AE2-E25C-4D8C-BE76-F012C327DE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A1FB27-7E06-4315-AD3C-EB205190E984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -119,6 +119,12 @@
   <si>
     <t>Sample Date
 August 23, 2022</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Annual Vacation</t>
   </si>
 </sst>
 </file>
@@ -290,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -306,6 +312,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -328,6 +335,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -682,27 +692,27 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -785,10 +795,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -799,9 +809,11 @@
     <col min="4" max="4" width="12.36328125" style="7" customWidth="1"/>
     <col min="5" max="5" width="13.81640625" style="7" customWidth="1"/>
     <col min="7" max="8" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.5" customHeight="1">
+    <row r="1" spans="1:14" ht="34.5" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -826,8 +838,13 @@
       <c r="H1" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="I1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="6" t="s">
         <v>24</v>
       </c>
@@ -852,22 +869,30 @@
       <c r="H2" s="8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="J4" s="19" t="s">
+      <c r="I2" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="L4" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="9"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="J5" s="21"/>
-      <c r="K5" s="22"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="L5" s="22"/>
+      <c r="M5" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="J4:K5"/>
+    <mergeCell ref="L4:M5"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{F0066729-EAC1-48F0-B928-B73C2B016E22}">
+      <formula1>"Annual Vacation, Sick"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
TC_04 - Absence script complete for requesting a single day in current month
</commit_message>
<xml_diff>
--- a/Input/UserDetails.xlsx
+++ b/Input/UserDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibmadmin\PycharmProjects\Workday\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A1FB27-7E06-4315-AD3C-EB205190E984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140048F4-7727-4E0D-AE7E-F21ECDB91EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -109,12 +109,6 @@
   </si>
   <si>
     <t>30</t>
-  </si>
-  <si>
-    <t>June 22, 2022</t>
-  </si>
-  <si>
-    <t>June 23, 2022</t>
   </si>
   <si>
     <t>Sample Date
@@ -125,6 +119,9 @@
   </si>
   <si>
     <t>Annual Vacation</t>
+  </si>
+  <si>
+    <t>June 28, 2022</t>
   </si>
 </sst>
 </file>
@@ -314,6 +311,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -335,9 +335,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -692,27 +689,27 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -798,7 +795,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -839,10 +836,10 @@
         <v>23</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+        <v>30</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="6" t="s">
@@ -864,25 +861,23 @@
         <v>1</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="L4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="L4" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="21"/>
+      <c r="M4" s="22"/>
       <c r="N4" s="9"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="L5" s="22"/>
-      <c r="M5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
TC_04 - Absence script complete for requesting a single day in different month and next year
</commit_message>
<xml_diff>
--- a/Input/UserDetails.xlsx
+++ b/Input/UserDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibmadmin\PycharmProjects\Workday\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140048F4-7727-4E0D-AE7E-F21ECDB91EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49270D30-6D76-48A3-A914-9D029CB7C9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -42,9 +42,6 @@
     <t>./Input/secret.txt</t>
   </si>
   <si>
-    <t>Create a secret.txt file inside Input folder and keep your password there. Please ensure secret.txt is added to gitignore file to avoid upload</t>
-  </si>
-  <si>
     <t>Shift</t>
   </si>
   <si>
@@ -111,23 +108,35 @@
     <t>30</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Annual Vacation</t>
+  </si>
+  <si>
+    <t>Vacation end date is only required when absence is for multiple days. Select Type from dropdown values.</t>
+  </si>
+  <si>
+    <t>Create a secret.txt file inside Input folder and keep your password there. Please ensure secret.txt is added to gitignore file to avoid public sharing.</t>
+  </si>
+  <si>
+    <t>For any absence put the value as 0</t>
+  </si>
+  <si>
     <t>Sample Date
-August 23, 2022</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Annual Vacation</t>
-  </si>
-  <si>
-    <t>June 28, 2022</t>
+December 22, 2022</t>
+  </si>
+  <si>
+    <t>January 22, 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mmmm\ [$-14009]d\,\ yyyy;@"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -159,7 +168,7 @@
       <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +193,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -293,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -314,6 +341,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -325,16 +353,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -655,7 +722,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:I6"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -689,27 +756,27 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="E4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14"/>
+      <c r="E4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="17"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="20"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -725,43 +792,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="3" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
@@ -785,17 +852,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:11">
+      <c r="J4" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="23"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="J5" s="24"/>
+      <c r="K5" s="25"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J4:K5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -804,84 +884,106 @@
     <col min="2" max="2" width="8.81640625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1796875" style="7" customWidth="1"/>
     <col min="4" max="4" width="12.36328125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" style="7" customWidth="1"/>
-    <col min="7" max="8" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="34.5" customHeight="1">
       <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="I1" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="12"/>
       <c r="I2" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="L4" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="22"/>
+      <c r="L4" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="27"/>
       <c r="N4" s="9"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="29"/>
+    </row>
+    <row r="7" spans="1:14" ht="14.5" customHeight="1">
+      <c r="K7" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="32"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="K8" s="33"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="35"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="K9" s="36"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="L4:M5"/>
+    <mergeCell ref="K7:N9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{F0066729-EAC1-48F0-B928-B73C2B016E22}">

</xml_diff>

<commit_message>
TC_04 - Absence script modified for requesting multiple days
</commit_message>
<xml_diff>
--- a/Input/UserDetails.xlsx
+++ b/Input/UserDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibmadmin\PycharmProjects\Workday\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49270D30-6D76-48A3-A914-9D029CB7C9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AABC1D5-DDBA-421C-AB7A-2170EC7AA033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>January 22, 2023</t>
+  </si>
+  <si>
+    <t>Single Day</t>
   </si>
 </sst>
 </file>
@@ -320,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -403,6 +406,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -875,7 +881,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -885,6 +891,7 @@
     <col min="3" max="3" width="11.1796875" style="7" customWidth="1"/>
     <col min="4" max="4" width="12.36328125" style="7" customWidth="1"/>
     <col min="5" max="5" width="13.08984375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.90625" customWidth="1"/>
     <col min="7" max="7" width="15.26953125" style="7" customWidth="1"/>
     <col min="8" max="8" width="14.7265625" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
@@ -938,8 +945,8 @@
       <c r="E2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="3">
-        <v>2</v>
+      <c r="F2" s="39" t="s">
+        <v>35</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>34</v>
@@ -985,9 +992,12 @@
     <mergeCell ref="L4:M5"/>
     <mergeCell ref="K7:N9"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{F0066729-EAC1-48F0-B928-B73C2B016E22}">
       <formula1>"Annual Vacation, Sick"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{1847EB2F-EB45-4604-955A-F4119EC7CE4F}">
+      <formula1>"Single Day, Multiple Days"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "TC_04 - Absence script modified for requesting multiple days"
This reverts commit e2faba7646160de15f405d24da0ed2991e60bab6.
</commit_message>
<xml_diff>
--- a/Input/UserDetails.xlsx
+++ b/Input/UserDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibmadmin\PycharmProjects\Workday\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AABC1D5-DDBA-421C-AB7A-2170EC7AA033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49270D30-6D76-48A3-A914-9D029CB7C9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>January 22, 2023</t>
-  </si>
-  <si>
-    <t>Single Day</t>
   </si>
 </sst>
 </file>
@@ -323,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -406,9 +403,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -881,7 +875,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -891,7 +885,6 @@
     <col min="3" max="3" width="11.1796875" style="7" customWidth="1"/>
     <col min="4" max="4" width="12.36328125" style="7" customWidth="1"/>
     <col min="5" max="5" width="13.08984375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="12.90625" customWidth="1"/>
     <col min="7" max="7" width="15.26953125" style="7" customWidth="1"/>
     <col min="8" max="8" width="14.7265625" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
@@ -945,8 +938,8 @@
       <c r="E2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="39" t="s">
-        <v>35</v>
+      <c r="F2" s="3">
+        <v>2</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>34</v>
@@ -992,12 +985,9 @@
     <mergeCell ref="L4:M5"/>
     <mergeCell ref="K7:N9"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{F0066729-EAC1-48F0-B928-B73C2B016E22}">
       <formula1>"Annual Vacation, Sick"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{1847EB2F-EB45-4604-955A-F4119EC7CE4F}">
-      <formula1>"Single Day, Multiple Days"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>